<commit_message>
feat: add some files
</commit_message>
<xml_diff>
--- a/3 Курс/МДК 02.03/Лабораторная работа 7/lab7_variant6.xlsx
+++ b/3 Курс/МДК 02.03/Лабораторная работа 7/lab7_variant6.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Secret\fork\Labwork\3 Курс\МДК 02.03\Лабораторная работа 7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBA1C7B8-99EE-40E6-880F-6F997451CA90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50CAA973-3F8C-47D2-B7C2-B7C8D9A18679}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28980" yWindow="7665" windowWidth="29160" windowHeight="15960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -166,14 +166,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -265,7 +258,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.10140943880005002"/>
+          <c:y val="0.20406277340332457"/>
+          <c:w val="0.88440320443112241"/>
+          <c:h val="0.47955016039661708"/>
+        </c:manualLayout>
+      </c:layout>
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
@@ -1457,30 +1460,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N42" sqref="N42"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.921875" customWidth="1"/>
-    <col min="2" max="2" width="24.921875" customWidth="1"/>
-    <col min="3" max="3" width="26.3046875" customWidth="1"/>
-    <col min="4" max="4" width="42.69140625" customWidth="1"/>
-    <col min="5" max="5" width="30.15234375" customWidth="1"/>
-    <col min="6" max="6" width="39.61328125" customWidth="1"/>
-    <col min="7" max="7" width="38.921875" customWidth="1"/>
-    <col min="8" max="8" width="30.921875" customWidth="1"/>
-    <col min="9" max="9" width="38.61328125" customWidth="1"/>
-    <col min="10" max="10" width="29.69140625" customWidth="1"/>
-    <col min="11" max="11" width="40.61328125" customWidth="1"/>
-    <col min="12" max="12" width="34.61328125" customWidth="1"/>
-    <col min="13" max="13" width="19.3828125" customWidth="1"/>
-    <col min="14" max="14" width="53.07421875" customWidth="1"/>
-    <col min="15" max="15" width="27.4609375" customWidth="1"/>
+    <col min="1" max="1" width="7.85546875" customWidth="1"/>
+    <col min="2" max="2" width="24.85546875" customWidth="1"/>
+    <col min="3" max="3" width="26.28515625" customWidth="1"/>
+    <col min="4" max="4" width="42.7109375" customWidth="1"/>
+    <col min="5" max="5" width="30.140625" customWidth="1"/>
+    <col min="6" max="6" width="39.5703125" customWidth="1"/>
+    <col min="7" max="7" width="38.85546875" customWidth="1"/>
+    <col min="8" max="8" width="30.85546875" customWidth="1"/>
+    <col min="9" max="9" width="38.5703125" customWidth="1"/>
+    <col min="10" max="10" width="29.7109375" customWidth="1"/>
+    <col min="11" max="11" width="40.5703125" customWidth="1"/>
+    <col min="12" max="12" width="34.5703125" customWidth="1"/>
+    <col min="13" max="13" width="19.42578125" customWidth="1"/>
+    <col min="14" max="14" width="53.140625" customWidth="1"/>
+    <col min="15" max="15" width="27.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>23</v>
       </c>
@@ -1527,7 +1530,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>2010</v>
       </c>
@@ -1574,7 +1577,7 @@
       </c>
       <c r="O2" s="4"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2011</v>
       </c>
@@ -1601,7 +1604,7 @@
         <v>-2</v>
       </c>
       <c r="H3" s="4">
-        <f t="shared" si="3"/>
+        <f>B3/$B$2*100</f>
         <v>99.989314526900671</v>
       </c>
       <c r="I3" s="4">
@@ -1633,7 +1636,7 @@
         <v>0.99989314526900674</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>2012</v>
       </c>
@@ -1692,7 +1695,7 @@
         <v>0.98626769970611805</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>2013</v>
       </c>
@@ -1751,7 +1754,7 @@
         <v>1.0012460721638314</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>2014</v>
       </c>
@@ -1810,7 +1813,7 @@
         <v>0.98917807477950326</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>2015</v>
       </c>
@@ -1869,7 +1872,7 @@
         <v>0.99830425031453418</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>2016</v>
       </c>
@@ -1928,7 +1931,7 @@
         <v>0.98575342465753424</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>2017</v>
       </c>
@@ -1987,7 +1990,7 @@
         <v>1.0015008337965536</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>2018</v>
       </c>
@@ -2046,7 +2049,7 @@
         <v>0.99295110173724821</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>2019</v>
       </c>
@@ -2105,7 +2108,7 @@
         <v>0.98485187255449969</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>2020</v>
       </c>
@@ -2164,7 +2167,7 @@
         <v>1.0028946024178444</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>2</v>
       </c>
@@ -2173,7 +2176,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -2182,7 +2185,7 @@
         <v>200088</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>20</v>
       </c>
@@ -2191,7 +2194,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -2200,7 +2203,7 @@
         <v>1187986</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -2209,7 +2212,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -2218,7 +2221,7 @@
         <v>-114.01818181818182</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>16</v>
       </c>
@@ -2227,7 +2230,7 @@
         <v>18873.927272727273</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>15</v>
       </c>
@@ -2236,7 +2239,7 @@
         <v>18189.81818181818</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>14</v>
       </c>
@@ -2245,7 +2248,7 @@
         <v>-104.7</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>13</v>
       </c>
@@ -2254,7 +2257,7 @@
         <v>99.426014473032666</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>12</v>
       </c>
@@ -2263,7 +2266,7 @@
         <v>-0.57398552696733418</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>11</v>
       </c>
@@ -2272,7 +2275,7 @@
         <v>1098</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>10</v>
       </c>
@@ -2281,7 +2284,7 @@
         <v>2.015248578744679</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>9</v>
       </c>
@@ -2290,7 +2293,7 @@
         <v>66.122200920306994</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>8</v>
       </c>
@@ -2299,7 +2302,7 @@
         <v>17505.709090909091</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>7</v>
       </c>
@@ -2308,7 +2311,7 @@
         <v>17391.69090909091</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>6</v>
       </c>
@@ -2317,7 +2320,7 @@
         <v>17439.586889988783</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>5</v>
       </c>
@@ -2326,7 +2329,7 @@
         <v>17571.8312918294</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>4</v>
       </c>
@@ -2335,7 +2338,7 @@
         <v>17325.568708170602</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
feat: add additional file
</commit_message>
<xml_diff>
--- a/3 Курс/МДК 02.03/Лабораторная работа 7/lab7_variant6.xlsx
+++ b/3 Курс/МДК 02.03/Лабораторная работа 7/lab7_variant6.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Secret\fork\Labwork\3 Курс\МДК 02.03\Лабораторная работа 7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50CAA973-3F8C-47D2-B7C2-B7C8D9A18679}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3988B47E-DFDE-4EED-8B02-BDDD52126560}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <si>
     <t>x</t>
   </si>
@@ -160,6 +160,66 @@
   </si>
   <si>
     <t>Цепной коэффициент роста</t>
+  </si>
+  <si>
+    <t>Для этого:</t>
+  </si>
+  <si>
+    <t>1. Рассчитать средний уровень ряда.</t>
+  </si>
+  <si>
+    <t>2. Рассчитать абсолютный прирост, темп роста и темп прироста для всех уровней и</t>
+  </si>
+  <si>
+    <t>средние значения этих показателей.</t>
+  </si>
+  <si>
+    <t>3. Провести аналитическое выравнивание динамического ряда методом</t>
+  </si>
+  <si>
+    <t>наименьших квадратов, т.е. функцию y = f(x), заданную таблично,</t>
+  </si>
+  <si>
+    <t>аппроксимировать многочленом первой степени y = P1</t>
+  </si>
+  <si>
+    <t>(x) = a1 + a2x;</t>
+  </si>
+  <si>
+    <t>4. Рассчитать точность полученной динамической модели (уравнения) ряда,</t>
+  </si>
+  <si>
+    <t>сделать прогноз на два года.</t>
+  </si>
+  <si>
+    <t>5. Определить колеблемость показателя и его устойчивость.</t>
+  </si>
+  <si>
+    <t>6. Показать на графике исходный и выровненный динамические ряды.</t>
+  </si>
+  <si>
+    <t>7. Средствами MS Excel построить точечную диаграмму по исходным табличным</t>
+  </si>
+  <si>
+    <t>данным, соответствующим своему варианту. Добавить линии тренда: линейный,</t>
+  </si>
+  <si>
+    <t>полиномиальный, экспоненциальный. Установить флаги «Показывать уравнение</t>
+  </si>
+  <si>
+    <t>на диаграмме», «Поместить на диаграмму величину достоверности</t>
+  </si>
+  <si>
+    <t>аппроксимации (R^2)». Для линейной линии тренда сравнить ее показатели с</t>
+  </si>
+  <si>
+    <t>рассчитанными аналитическим путем коэффициентами. Сделать вывод о том,</t>
+  </si>
+  <si>
+    <t>какая из линий тренда лучше аппроксимирует исходные данные.</t>
+  </si>
+  <si>
+    <t>8. Сделать выводы по работе.</t>
   </si>
 </sst>
 </file>
@@ -780,8 +840,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="2.4182923071933579E-2"/>
-                  <c:y val="-0.25833520809898763"/>
+                  <c:x val="1.6405838033015452E-3"/>
+                  <c:y val="-0.29745552639253425"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -1099,15 +1159,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>238125</xdr:colOff>
+      <xdr:colOff>796019</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:rowOff>108856</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>1066800</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:colOff>1409701</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>133349</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1135,15 +1195,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>238125</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:colOff>798739</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>125185</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>1066800</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>657225</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1458,21 +1518,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O33"/>
+  <dimension ref="A1:O40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.85546875" customWidth="1"/>
-    <col min="2" max="2" width="24.85546875" customWidth="1"/>
+    <col min="2" max="2" width="30.42578125" customWidth="1"/>
     <col min="3" max="3" width="26.28515625" customWidth="1"/>
     <col min="4" max="4" width="42.7109375" customWidth="1"/>
     <col min="5" max="5" width="30.140625" customWidth="1"/>
-    <col min="6" max="6" width="39.5703125" customWidth="1"/>
-    <col min="7" max="7" width="38.85546875" customWidth="1"/>
+    <col min="6" max="6" width="44.7109375" customWidth="1"/>
+    <col min="7" max="7" width="44" customWidth="1"/>
     <col min="8" max="8" width="30.85546875" customWidth="1"/>
     <col min="9" max="9" width="38.5703125" customWidth="1"/>
     <col min="10" max="10" width="29.7109375" customWidth="1"/>
@@ -2194,7 +2254,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -2203,7 +2263,7 @@
         <v>1187986</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -2212,7 +2272,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -2220,8 +2280,11 @@
         <f>($C$18*$C$17 - $C$14*$C$15)/($C$18*$C$16 - $C$14^2)</f>
         <v>-114.01818181818182</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E19" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>16</v>
       </c>
@@ -2229,8 +2292,11 @@
         <f>($C$15 - $C$19*$C$14)/$C$18</f>
         <v>18873.927272727273</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>15</v>
       </c>
@@ -2238,8 +2304,11 @@
         <f>AVERAGE(B2:B12)</f>
         <v>18189.81818181818</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E21" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>14</v>
       </c>
@@ -2247,8 +2316,11 @@
         <f>(B12-B2)/($C$18-1)</f>
         <v>-104.7</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E22" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>13</v>
       </c>
@@ -2256,8 +2328,11 @@
         <f>GEOMEAN(O3:O12)*100</f>
         <v>99.426014473032666</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E23" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>12</v>
       </c>
@@ -2265,8 +2340,11 @@
         <f>$C$23 - 100</f>
         <v>-0.57398552696733418</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E24" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>11</v>
       </c>
@@ -2274,8 +2352,11 @@
         <f>MAX(B2:B12)-MIN(B2:B12)</f>
         <v>1098</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E25" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>10</v>
       </c>
@@ -2284,7 +2365,7 @@
         <v>2.015248578744679</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>9</v>
       </c>
@@ -2292,8 +2373,11 @@
         <f>SQRT(SUM(N2:N12)/$C$18)</f>
         <v>66.122200920306994</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E27" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>8</v>
       </c>
@@ -2302,7 +2386,7 @@
         <v>17505.709090909091</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>7</v>
       </c>
@@ -2310,8 +2394,11 @@
         <f>$C$20 + $C$19*($C$18+2)</f>
         <v>17391.69090909091</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E29" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>6</v>
       </c>
@@ -2319,8 +2406,11 @@
         <f>$C$28 - $C$27</f>
         <v>17439.586889988783</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E30" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>5</v>
       </c>
@@ -2328,8 +2418,11 @@
         <f>$C$28 + $C$27</f>
         <v>17571.8312918294</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E31" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>4</v>
       </c>
@@ -2337,14 +2430,55 @@
         <f>$C$29 - $C$27</f>
         <v>17325.568708170602</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E32" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>3</v>
       </c>
       <c r="C33" s="1">
         <f>$C$29 + $C$27</f>
         <v>17457.813110011219</v>
+      </c>
+      <c r="E33" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E34" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E35" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E36" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E37" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E38" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E39" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E40" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>